<commit_message>
feat: Enhance chemical and sample import functionality
- Updated  in   for better matching with .
- Added support for importing  and  fields in XLSX and SDF template files.
- Refactored SDF files to align with updated field name
</commit_message>
<xml_diff>
--- a/public/xlsx/chemical_import_example.xlsx
+++ b/public/xlsx/chemical_import_example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49172\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49172\Downloads\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCFB9C6-CC92-4FA4-B8C7-C3DD4EA1B066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690DD84D-354C-4082-8EA9-42DED9E8C4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28020" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample_chemicals" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
   <si>
     <t>decoupled</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>location</t>
-  </si>
-  <si>
-    <t>secret</t>
   </si>
   <si>
     <t>dry solvent</t>
@@ -296,6 +293,21 @@
   </si>
   <si>
     <t>4.0 g/ml</t>
+  </si>
+  <si>
+    <t>2023-05-09</t>
+  </si>
+  <si>
+    <t>2029-05-09</t>
+  </si>
+  <si>
+    <t>2022-04-09</t>
+  </si>
+  <si>
+    <t>is top secret</t>
+  </si>
+  <si>
+    <t>1.2</t>
   </si>
 </sst>
 </file>
@@ -365,13 +377,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -708,8 +721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:X1048576"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +744,7 @@
     <col min="16" max="16" width="255" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" customWidth="1"/>
     <col min="20" max="20" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="31.85546875" bestFit="1" customWidth="1"/>
@@ -769,167 +782,167 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AC1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BB1" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="BB1" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:54" ht="150" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -937,46 +950,46 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
         <v>48</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>49</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>50</v>
       </c>
-      <c r="H2" t="s">
-        <v>51</v>
-      </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J2" t="s">
-        <v>79</v>
-      </c>
-      <c r="K2">
-        <v>1.2</v>
+        <v>78</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="L2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" t="s">
+        <v>79</v>
+      </c>
+      <c r="P2" t="s">
         <v>52</v>
       </c>
-      <c r="O2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P2" t="s">
-        <v>53</v>
-      </c>
       <c r="Q2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="S2" t="b">
         <v>0</v>
@@ -991,55 +1004,55 @@
         <v>70</v>
       </c>
       <c r="W2" t="s">
+        <v>53</v>
+      </c>
+      <c r="X2" t="s">
         <v>54</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>55</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>56</v>
       </c>
-      <c r="Z2" t="s">
-        <v>57</v>
-      </c>
       <c r="AA2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB2" t="s">
         <v>76</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>77</v>
       </c>
       <c r="AC2">
         <v>150</v>
       </c>
       <c r="AD2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AE2" s="1">
-        <v>45061</v>
-      </c>
-      <c r="AF2" s="1">
-        <v>54789</v>
-      </c>
-      <c r="AG2" s="1">
-        <v>45065</v>
+        <v>77</v>
+      </c>
+      <c r="AE2" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF2" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="AH2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI2" t="s">
         <v>58</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AK2" t="s">
         <v>59</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AM2" t="s">
         <v>60</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>61</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>62</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>63</v>
       </c>
       <c r="AP2">
         <v>1</v>
@@ -1048,16 +1061,16 @@
         <v>2</v>
       </c>
       <c r="AR2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS2" t="s">
         <v>64</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>65</v>
       </c>
-      <c r="AT2" t="s">
-        <v>66</v>
-      </c>
       <c r="BB2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>